<commit_message>
Buffer range  --- station number Station name   ---need_revised_row    return  'name' list
</commit_message>
<xml_diff>
--- a/notebooks/need_revised_row.xlsx
+++ b/notebooks/need_revised_row.xlsx
@@ -455,7 +455,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 365436
+route                                                     bus
+to                                      Amsterdam, Louweshoek
+name        Bus 18: Amsterdam Centraal Station =&gt; Amsterda...
+ref                                                        18
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.900265 52.3797248, 4.89945...
+Name: 2, dtype: object</t>
         </is>
       </c>
     </row>
@@ -476,7 +484,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 364660
+route                                                     bus
+to                                    Amsterdam, Nolensstraat
+name        Bus 21: Amsterdam Centraal Station =&gt; Amsterda...
+ref                                                        21
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.900265 52.3797248, 4.89945...
+Name: 5, dtype: object</t>
         </is>
       </c>
     </row>
@@ -497,28 +513,60 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                8456140
+route                                                     bus
+to                                     Amsterdam, Noorderpark
+name        Bus 34: Amsterdam Olof Palmeplein =&gt; Amsterdam...
+ref                                                        34
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9401433 52.396837, 4.94000...
+Name: 8, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                8456179
+route                                                     bus
+to                                 Amsterdam, Olof Palmeplein
+name        Bus 34: Amsterdam Noorderpark =&gt; Amsterdam Olo...
+ref                                                        34
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9193382 52.3892587, 4.9192...
+Name: 9, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                8456882
+route                                                     bus
+to                                  Amsterdam Olof Palmeplein
+name        Bus 35: Amsterdam Molenwijk =&gt; Amsterdam Olof ...
+ref                                                        35
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8936702 52.4180657, 4.8937...
+Name: 10, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                8456944
+route                                                     bus
+to                                        Amsterdam Molenwijk
+name        Bus 35: Amsterdam Olof Palmeplein =&gt; Amsterdam...
+ref                                                        35
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9401433 52.396837, 4.94000...
+Name: 11, dtype: object</t>
         </is>
       </c>
     </row>
@@ -553,7 +601,15 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                8461307
+route                                                     bus
+to                                Amsterdam Metaalbewerkerweg
+name        Bus 38: Amsterdam Station Noord =&gt; Amsterdam B...
+ref                                                        38
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9333669 52.4019911, 4.9332...
+Name: 16, dtype: object</t>
         </is>
       </c>
     </row>
@@ -567,21 +623,45 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                4539112
+route                                                     bus
+to                                    Amsterdam Amstelstation
+name        Bus 40: Amsterdam Muiderpoortstation =&gt; Amster...
+ref                                                        40
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9337209 52.3610843, 4.9339...
+Name: 18, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                  73789
+route                                                     bus
+to                               Amsterdam Muiderpoortstation
+name        Bus 40: Amsterdam Amstelstation =&gt; Amsterdam M...
+ref                                                        40
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9186931 52.3461675, 4.9186...
+Name: 19, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 365785
+route                                                     bus
+to                             Amsterdam, Station Holendrecht
+name        Bus 41: Amsterdam Muiderpoortstation =&gt; Amster...
+ref                                                        41
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9771905 52.3236949, 4.9773...
+Name: 20, dtype: object</t>
         </is>
       </c>
     </row>
@@ -609,7 +689,15 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                4542861
+route                                                     bus
+to                            Amsterdam Station Bijlmer ArenA
+name        Bus 44: Diemen Noord =&gt; Amsterdam Station Bijl...
+ref                                                        44
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9663154 52.3440833, 4.9663...
+Name: 24, dtype: object</t>
         </is>
       </c>
     </row>
@@ -623,14 +711,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 365789
+route                                                     bus
+to                            Amsterdam Station Bijlmer ArenA
+name        Bus 47: Amsterdam Station Holendrecht =&gt; Amste...
+ref                                                        47
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9492523 52.3131284, 4.9493...
+Name: 26, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 365788
+route                                                     bus
+to                              Amsterdam Station Holendrecht
+name        Bus 47: Amsterdam Station Bijlmer ArenA =&gt; Ams...
+ref                                                        47
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.947369 52.3111419, 4.94752...
+Name: 27, dtype: object</t>
         </is>
       </c>
     </row>
@@ -644,35 +748,75 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                4543993
+route                                                     bus
+to                                    Amsterdam, Koivistokade
+name        Bus 48: Amsterdam Centraal Station =&gt; Amsterda...
+ref                                                        48
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9006338 52.3795871, 4.9002...
+Name: 29, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 365790
+route                                                     bus
+to                                              Weesp Station
+name        Bus 49: Amsterdam Station Bijlmer ArenA =&gt; Wee...
+ref                                                        49
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9474141 52.3110955, 4.9475...
+Name: 30, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                4547026
+route                                                     bus
+to                            Amsterdam Station Bijlmer ArenA
+name        Bus 49: Weesp Station =&gt; Amsterdam Station Bij...
+ref                                                        49
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.9919942 52.3142796, 4.9921...
+Name: 31, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 375858
+route                                                     bus
+to                                Amsterdam Osdorpplein Noord
+name        Bus 61: Amsterdam Station Sloterdijk =&gt; Amster...
+ref                                                        61
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8387533 52.3881185, 4.8386...
+Name: 32, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 365437
+route                                                     bus
+to                               Amsterdam Station Sloterdijk
+name        Bus 61: Amsterdam Osdorpplein =&gt; Amsterdam Sta...
+ref                                                        61
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8051399 52.3602896, 4.8047...
+Name: 33, dtype: object</t>
         </is>
       </c>
     </row>
@@ -693,14 +837,30 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                4552870
+route                                                     bus
+to                                 Amsterdam Station Lelylaan
+name        Bus 63: Osdorp De Aker =&gt; Amsterdam Station Le...
+ref                                                        63
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.7745693 52.3543998, 4.7753...
+Name: 36, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 375860
+route                                                     bus
+to                                             Osdorp De Aker
+name        Bus 63: Amsterdam Station Lelylaan =&gt; Osdorp D...
+ref                                                        63
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8343566 52.3566723, 4.8343...
+Name: 37, dtype: object</t>
         </is>
       </c>
     </row>
@@ -714,7 +874,15 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                4552871
+route                                                     bus
+to                                       Amsterdam, KNSM-laan
+name        Bus 65: Amsterdam Station Zuid =&gt; Amsterdam KN...
+ref                                                        65
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8768122 52.3431691, 4.8768...
+Name: 39, dtype: object</t>
         </is>
       </c>
     </row>
@@ -735,28 +903,60 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                5860193
+route                                                     bus
+to                             Amsterdam, John M. Keynesplein
+name        Bus 68: Amsterdam Henk Sneevlietweg =&gt; Amsterd...
+ref                                                        68
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8330587 52.3457424, 4.8328...
+Name: 42, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                6096663
+route                                                     bus
+to                               Amsterdam, Henk Sneevlietweg
+name        Bus 68: Amsterdam Riekerpolder =&gt; Amsterdam He...
+ref                                                        68
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.824444 52.340413, 4.824449...
+Name: 43, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                               11720818
+route                                                     bus
+to                               Amsterdam, Henk Sneevlietweg
+name        Bus 68: Amsterdam Riekerpolder =&gt; Amsterdam He...
+ref                                                        68
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8252211 52.340147, 4.82543...
+Name: 44, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                               11720819
+route                                                     bus
+to                             Amsterdam, John M. Keynesplein
+name        Bus 68: Amsterdam Henk Sneevlietweg =&gt; Amsterd...
+ref                                                        68
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8330587 52.3457424, 4.8328...
+Name: 45, dtype: object</t>
         </is>
       </c>
     </row>
@@ -770,7 +970,15 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 375862
+route                                                     bus
+to                                       Amsterdam, Abberdaan
+name        Bus 231: Amsterdam Station Sloterdijk =&gt; Amste...
+ref                                                       231
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8388353 52.3874811, 4.8387...
+Name: 47, dtype: object</t>
         </is>
       </c>
     </row>
@@ -819,14 +1027,30 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                               11730321
+route                                                     bus
+to                             Amsterdam, John M. Keynesplein
+name        Bus 267: Amsterdam Sloten =&gt; Amsterdam Riekerp...
+ref                                                       267
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8143076 52.3354966, 4.8143...
+Name: 54, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                 375866
+route                                                     bus
+to                                    Schiphol, Airport/Plaza
+name        Bus 369: Amsterdam Station Sloterdijk =&gt; Schip...
+ref                                                       369
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.838741 52.38822, 4.838631 ...
+Name: 55, dtype: object</t>
         </is>
       </c>
     </row>
@@ -840,42 +1064,90 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                6900423
+route                                                     bus
+to                               Amsterdam Gustav Mahlerplein
+name        Bus 461: Amsterdam Gelderlandplein NO =&gt; Amste...
+ref                                                       461
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8791445 52.3318593, 4.8791...
+Name: 57, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                6900422
+route                                                     bus
+to                               Amsterdam Gelderlandplein NO
+name        Bus 461: Amsterdam Gustav Mahlerplein =&gt; Amste...
+ref                                                       461
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8731084 52.336651, 4.87323...
+Name: 58, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                6900421
+route                                                     bus
+to                                       Amsterdam, Bolestein
+name        Bus 463: Amsterdam Gelderlandplein Oost =&gt; Ams...
+ref                                                       463
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8794156 52.3308129, 4.8794...
+Name: 59, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                                6900419
+route                                                     bus
+to                           Amsterdam, Gelderlandplein Noord
+name        Bus 463: Amsterdam Bolestein =&gt; Amsterdam Geld...
+ref                                                       463
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8596699 52.3249815, 4.8596...
+Name: 60, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                               11730318
+route                                                     bus
+to                                    Amsterdam, De Boelelaan
+name        Bus 464: Amsterdam De Boelelaan/De Klencke =&gt; ...
+ref                                                       464
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8873203 52.3343831, 4.8875...
+Name: 61, dtype: object</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>no need to revise</t>
+          <t>osm_id                                               11730319
+route                                                     bus
+to                                    Amsterdam, De Boelelaan
+name        Bus 464: Amsterdam Gelderlandplein NO =&gt; Amste...
+ref                                                       464
+network                                Stadsvervoer Amsterdam
+service                                                  None
+geometry    MULTILINESTRING ((4.8791445 52.3318593, 4.8791...
+Name: 62, dtype: object</t>
         </is>
       </c>
     </row>

</xml_diff>